<commit_message>
update with changed datagram
</commit_message>
<xml_diff>
--- a/Deps/i2c datagram.xlsx
+++ b/Deps/i2c datagram.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex lorman\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Main Storage\Dropbox Offlining\2006 4Runner\New Switch Rack\4runner-lights\Deps\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
   <si>
     <t xml:space="preserve">Datagram </t>
   </si>
@@ -35,36 +35,18 @@
     <t>March 4 17</t>
   </si>
   <si>
-    <t>TFourR</t>
-  </si>
-  <si>
     <t>Wire Byte</t>
   </si>
   <si>
-    <t>Upper-&gt;</t>
-  </si>
-  <si>
-    <t>Lower</t>
-  </si>
-  <si>
-    <t>Lower-&gt;</t>
-  </si>
-  <si>
     <t>(who is sending)</t>
   </si>
   <si>
-    <t>Upper</t>
-  </si>
-  <si>
     <t>(who is the target</t>
   </si>
   <si>
     <t>Intro</t>
   </si>
   <si>
-    <t>T/</t>
-  </si>
-  <si>
     <t>Program time</t>
   </si>
   <si>
@@ -98,64 +80,91 @@
     <t>High State</t>
   </si>
   <si>
-    <t>CH1</t>
-  </si>
-  <si>
     <t>Ch1</t>
   </si>
   <si>
     <t>Ch1 Status</t>
   </si>
   <si>
-    <t>CH2</t>
-  </si>
-  <si>
     <t>Ch2</t>
   </si>
   <si>
-    <t>CH3</t>
-  </si>
-  <si>
     <t>ch3</t>
   </si>
   <si>
     <t>Ch3</t>
   </si>
   <si>
-    <t>CH4</t>
-  </si>
-  <si>
     <t>Ch4</t>
   </si>
   <si>
-    <t>CH5</t>
-  </si>
-  <si>
     <t>Ch5</t>
   </si>
   <si>
-    <t>CH6</t>
-  </si>
-  <si>
     <t>Ch6</t>
   </si>
   <si>
-    <t>i2C formatting</t>
-  </si>
-  <si>
-    <t>1 is upper</t>
-  </si>
-  <si>
-    <t>2 is lower</t>
-  </si>
-  <si>
-    <t>V/</t>
-  </si>
-  <si>
     <t>Voltage</t>
   </si>
   <si>
     <t>Voltage x100</t>
+  </si>
+  <si>
+    <t>TFourR/</t>
+  </si>
+  <si>
+    <t>T-</t>
+  </si>
+  <si>
+    <t>V-</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>Spacer</t>
+  </si>
+  <si>
+    <t>1234/</t>
+  </si>
+  <si>
+    <t>1/</t>
+  </si>
+  <si>
+    <t>0/</t>
+  </si>
+  <si>
+    <t>CH1-</t>
+  </si>
+  <si>
+    <t>CH2-</t>
+  </si>
+  <si>
+    <t>CH3-</t>
+  </si>
+  <si>
+    <t>CH4-</t>
+  </si>
+  <si>
+    <t>CH5-</t>
+  </si>
+  <si>
+    <t>CH6-</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t>{address}</t>
+  </si>
+  <si>
+    <t>Serial formatting (strict breaklines)</t>
+  </si>
+  <si>
+    <t>TFourR/Upper &gt;Lower/T-4294967295/V-1234/I1/L1/H1/CH1-255/CH2-255/CH3-255/CH4-255/CH5-255/CH6-255/</t>
+  </si>
+  <si>
+    <t>Demarcation</t>
   </si>
 </sst>
 </file>
@@ -473,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y8"/>
+  <dimension ref="A1:Z10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,12 +495,13 @@
     <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -502,291 +512,322 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
+        <f>A3+1</f>
         <v>2</v>
       </c>
       <c r="C3">
+        <f t="shared" ref="C3:Z3" si="0">B3+1</f>
         <v>3</v>
       </c>
       <c r="D3">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E3">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="F3">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="G3">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="H3">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="I3">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="J3">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="K3">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="L3">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="M3">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="N3">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="O3">
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="P3">
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="Q3">
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="R3">
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="S3">
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="T3">
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="U3">
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="V3">
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="W3">
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="X3">
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="Y3">
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
+      <c r="Z3">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E4">
         <v>12345789</v>
       </c>
       <c r="F4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O4" t="s">
+        <v>36</v>
+      </c>
+      <c r="P4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>37</v>
+      </c>
+      <c r="R4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S4" t="s">
+        <v>38</v>
+      </c>
+      <c r="T4" t="s">
+        <v>35</v>
+      </c>
+      <c r="U4" t="s">
+        <v>39</v>
+      </c>
+      <c r="V4" t="s">
+        <v>35</v>
+      </c>
+      <c r="W4" t="s">
+        <v>40</v>
+      </c>
+      <c r="X4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y4" t="s">
         <v>41</v>
       </c>
-      <c r="G4">
-        <v>1234</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="Z4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5" t="s">
         <v>16</v>
       </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5" t="s">
+        <v>18</v>
+      </c>
+      <c r="P5">
+        <v>255</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>20</v>
+      </c>
+      <c r="R5">
+        <v>255</v>
+      </c>
+      <c r="S5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T5">
+        <v>255</v>
+      </c>
+      <c r="U5" t="s">
+        <v>23</v>
+      </c>
+      <c r="V5">
+        <v>255</v>
+      </c>
+      <c r="W5" t="s">
+        <v>24</v>
+      </c>
+      <c r="X5">
+        <v>255</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z5">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O6" t="s">
         <v>19</v>
       </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4" t="s">
-        <v>15</v>
-      </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="N4" t="s">
+      <c r="Q6" t="s">
+        <v>20</v>
+      </c>
+      <c r="S6" t="s">
+        <v>22</v>
+      </c>
+      <c r="U6" t="s">
+        <v>23</v>
+      </c>
+      <c r="W6" t="s">
         <v>24</v>
       </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4" t="s">
-        <v>29</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4" t="s">
-        <v>32</v>
-      </c>
-      <c r="U4">
-        <v>0</v>
-      </c>
-      <c r="V4" t="s">
-        <v>34</v>
-      </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
-      <c r="X4" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y4">
-        <v>0</v>
+      <c r="Y6" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" t="s">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
         <v>42</v>
       </c>
-      <c r="G5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5" t="s">
-        <v>20</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5" t="s">
-        <v>22</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5" t="s">
-        <v>25</v>
-      </c>
-      <c r="O5">
-        <v>255</v>
-      </c>
-      <c r="P5" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q5">
-        <v>255</v>
-      </c>
-      <c r="R5" t="s">
-        <v>30</v>
-      </c>
-      <c r="S5">
-        <v>255</v>
-      </c>
-      <c r="T5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U5">
-        <v>255</v>
-      </c>
-      <c r="V5" t="s">
-        <v>35</v>
-      </c>
-      <c r="W5">
-        <v>255</v>
-      </c>
-      <c r="X5" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y5">
-        <v>255</v>
-      </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" t="s">
-        <v>21</v>
-      </c>
-      <c r="L6" t="s">
-        <v>23</v>
-      </c>
-      <c r="N6" t="s">
-        <v>26</v>
-      </c>
-      <c r="P6" t="s">
-        <v>28</v>
-      </c>
-      <c r="R6" t="s">
-        <v>31</v>
-      </c>
-      <c r="T6" t="s">
-        <v>33</v>
-      </c>
-      <c r="V6" t="s">
-        <v>35</v>
-      </c>
-      <c r="X6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>40</v>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>